<commit_message>
updated sensitivity analysis w new costs
</commit_message>
<xml_diff>
--- a/CBA (3) v2.xlsx
+++ b/CBA (3) v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanelmaheinonen/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A8E4B77-CA68-694B-85C4-14122FC9EE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683AA313-CD09-C849-AFD6-482D1D357621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28020" windowHeight="15580" xr2:uid="{CB19214C-161C-4FCD-BB74-FBBD26C9B7EC}"/>
+    <workbookView xWindow="-3400" yWindow="500" windowWidth="28020" windowHeight="15580" xr2:uid="{CB19214C-161C-4FCD-BB74-FBBD26C9B7EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tunnel" sheetId="1" r:id="rId1"/>
@@ -309,7 +309,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="140">
   <si>
     <t>Weekly benefits</t>
   </si>
@@ -1427,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D083A40F-175A-4EEC-B4D7-09BE1D9F546C}">
-  <dimension ref="A1:R134"/>
+  <dimension ref="A1:R139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="106" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2205,7 +2205,7 @@
       </c>
       <c r="C45" s="30"/>
       <c r="D45" s="31">
-        <f>SUM(B74:B134)</f>
+        <f>SUM(B79:B139)</f>
         <v>2884783680.2135434</v>
       </c>
     </row>
@@ -2344,677 +2344,731 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
-      <c r="B62" s="23"/>
+      <c r="B62" s="53"/>
       <c r="C62" s="51"/>
     </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B63" s="53"/>
+      <c r="C63" s="51"/>
+    </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="8"/>
+      <c r="B64" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C64" s="37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="8"/>
+      <c r="B65">
+        <v>90</v>
+      </c>
+      <c r="C65" s="51">
+        <f>B48</f>
+        <v>2.1980841979930288</v>
+      </c>
+      <c r="D65" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="8"/>
+      <c r="B66">
+        <v>50</v>
+      </c>
+      <c r="C66">
+        <f t="dataTable" ref="C66:C67" dt2D="0" dtr="0" r1="O37" ca="1"/>
+        <v>2.189928935838926</v>
+      </c>
+      <c r="D66" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="8"/>
+      <c r="B67">
+        <v>185</v>
+      </c>
+      <c r="C67">
+        <v>2.2174529456090255</v>
+      </c>
+      <c r="D67" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C69" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="8" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B65">
+      <c r="B70">
         <f>H38</f>
         <v>14.4</v>
       </c>
-      <c r="C65" s="52">
+      <c r="C70" s="52">
         <f>B48</f>
         <v>2.1980841979930288</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="8" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="B66">
+      <c r="B71">
         <v>20.8</v>
       </c>
-      <c r="C66" s="52">
-        <f t="dataTable" ref="C66" dt2D="0" dtr="0" r1="H38"/>
+      <c r="C71" s="52">
+        <f t="dataTable" ref="C71" dt2D="0" dtr="0" r1="H38"/>
         <v>3.1524764050829881</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>73</v>
       </c>
-      <c r="B71" s="23">
+      <c r="B76" s="23">
         <f>H29</f>
         <v>6.1500000000000001E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>74</v>
       </c>
-      <c r="B72" s="45">
+      <c r="B77" s="45">
         <f>H13</f>
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>75</v>
       </c>
-      <c r="B73" s="25" t="s">
+      <c r="B78" s="25" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
         <v>0</v>
       </c>
-      <c r="B74" s="26">
-        <f>$D$43*(1+$B$72)^-A74*(1+$B$71)^A74</f>
+      <c r="B79" s="26">
+        <f>$D$43*(1+$B$77)^-A79*(1+$B$76)^A79</f>
         <v>78283144.727272704</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80">
         <v>1</v>
       </c>
-      <c r="B75" s="26">
-        <f t="shared" ref="B75:B105" si="2">$D$43*(1+$B$72)^-A75*(1+$B$71)^A75</f>
+      <c r="B80" s="26">
+        <f>$D$43*(1+$B$77)^-A80*(1+$B$76)^A80</f>
         <v>76843498.602288246</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>2</v>
-      </c>
-      <c r="B76" s="26">
-        <f t="shared" si="2"/>
-        <v>75430327.920675427</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <f>A76+1</f>
-        <v>3</v>
-      </c>
-      <c r="B77" s="26">
-        <f t="shared" si="2"/>
-        <v>74043145.792573258</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <f t="shared" ref="A78:A134" si="3">A77+1</f>
-        <v>4</v>
-      </c>
-      <c r="B78" s="26">
-        <f t="shared" si="2"/>
-        <v>72681474.28214401</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="B79" s="26">
-        <f t="shared" si="2"/>
-        <v>71344844.242906526</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="B80" s="26">
-        <f t="shared" si="2"/>
-        <v>70032795.156097963</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81">
-        <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B81" s="26">
-        <f t="shared" si="2"/>
-        <v>68744874.972007781</v>
+        <f>$D$43*(1+$B$77)^-A81*(1+$B$76)^A81</f>
+        <v>75430327.920675427</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82">
-        <f t="shared" si="3"/>
-        <v>8</v>
+        <f>A81+1</f>
+        <v>3</v>
       </c>
       <c r="B82" s="26">
-        <f t="shared" si="2"/>
-        <v>67480639.954229891</v>
+        <f>$D$43*(1+$B$77)^-A82*(1+$B$76)^A82</f>
+        <v>74043145.792573258</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83">
-        <f t="shared" si="3"/>
-        <v>9</v>
+        <f t="shared" ref="A83:A139" si="2">A82+1</f>
+        <v>4</v>
       </c>
       <c r="B83" s="26">
-        <f t="shared" si="2"/>
-        <v>66239654.526778951</v>
+        <f>$D$43*(1+$B$77)^-A83*(1+$B$76)^A83</f>
+        <v>72681474.28214401</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84">
-        <f t="shared" si="3"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="B84" s="26">
-        <f t="shared" si="2"/>
-        <v>65021491.124018192</v>
+        <f>$D$43*(1+$B$77)^-A84*(1+$B$76)^A84</f>
+        <v>71344844.242906526</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85">
-        <f t="shared" si="3"/>
-        <v>11</v>
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="B85" s="26">
-        <f t="shared" si="2"/>
-        <v>63825730.043347217</v>
+        <f>$D$43*(1+$B$77)^-A85*(1+$B$76)^A85</f>
+        <v>70032795.156097963</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86">
-        <f t="shared" si="3"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="B86" s="26">
-        <f t="shared" si="2"/>
-        <v>62651959.30059886</v>
+        <f>$D$43*(1+$B$77)^-A86*(1+$B$76)^A86</f>
+        <v>68744874.972007781</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87">
-        <f t="shared" si="3"/>
-        <v>13</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="B87" s="26">
-        <f t="shared" si="2"/>
-        <v>61499774.488095157</v>
+        <f>$D$43*(1+$B$77)^-A87*(1+$B$76)^A87</f>
+        <v>67480639.954229891</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88">
-        <f t="shared" si="3"/>
-        <v>14</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="B88" s="26">
-        <f t="shared" si="2"/>
-        <v>60368778.635314107</v>
+        <f>$D$43*(1+$B$77)^-A88*(1+$B$76)^A88</f>
+        <v>66239654.526778951</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89">
-        <f t="shared" si="3"/>
-        <v>15</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="B89" s="26">
-        <f t="shared" si="2"/>
-        <v>59258582.072118327</v>
+        <f>$D$43*(1+$B$77)^-A89*(1+$B$76)^A89</f>
+        <v>65021491.124018192</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90">
-        <f>A89+1</f>
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="B90" s="26">
-        <f t="shared" si="2"/>
-        <v>58168802.294499375</v>
+        <f>$D$43*(1+$B$77)^-A90*(1+$B$76)^A90</f>
+        <v>63825730.043347217</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91">
-        <f t="shared" si="3"/>
-        <v>17</v>
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="B91" s="26">
-        <f t="shared" si="2"/>
-        <v>57099063.832790792</v>
+        <f>$D$43*(1+$B$77)^-A91*(1+$B$76)^A91</f>
+        <v>62651959.30059886</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92">
-        <f t="shared" si="3"/>
-        <v>18</v>
+        <f t="shared" si="2"/>
+        <v>13</v>
       </c>
       <c r="B92" s="26">
-        <f t="shared" si="2"/>
-        <v>56048998.122304827</v>
+        <f>$D$43*(1+$B$77)^-A92*(1+$B$76)^A92</f>
+        <v>61499774.488095157</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93">
-        <f t="shared" si="3"/>
-        <v>19</v>
+        <f t="shared" si="2"/>
+        <v>14</v>
       </c>
       <c r="B93" s="26">
-        <f t="shared" si="2"/>
-        <v>55018243.376348302</v>
+        <f>$D$43*(1+$B$77)^-A93*(1+$B$76)^A93</f>
+        <v>60368778.635314107</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f t="shared" si="2"/>
+        <v>15</v>
       </c>
       <c r="B94" s="26">
-        <f t="shared" si="2"/>
-        <v>54006444.461573519</v>
+        <f>$D$43*(1+$B$77)^-A94*(1+$B$76)^A94</f>
+        <v>59258582.072118327</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95">
-        <f t="shared" si="3"/>
-        <v>21</v>
+        <f>A94+1</f>
+        <v>16</v>
       </c>
       <c r="B95" s="26">
-        <f t="shared" si="2"/>
-        <v>53013252.775621668</v>
+        <f>$D$43*(1+$B$77)^-A95*(1+$B$76)^A95</f>
+        <v>58168802.294499375</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96">
-        <f t="shared" si="3"/>
-        <v>22</v>
+        <f t="shared" si="2"/>
+        <v>17</v>
       </c>
       <c r="B96" s="26">
-        <f t="shared" si="2"/>
-        <v>52038326.127016336</v>
+        <f>$D$43*(1+$B$77)^-A96*(1+$B$76)^A96</f>
+        <v>57099063.832790792</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97">
-        <f t="shared" si="3"/>
-        <v>23</v>
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
       <c r="B97" s="26">
-        <f t="shared" si="2"/>
-        <v>51081328.617265843</v>
+        <f>$D$43*(1+$B$77)^-A97*(1+$B$76)^A97</f>
+        <v>56048998.122304827</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98">
-        <f t="shared" si="3"/>
-        <v>24</v>
+        <f t="shared" si="2"/>
+        <v>19</v>
       </c>
       <c r="B98" s="26">
-        <f t="shared" si="2"/>
-        <v>50141930.525133699</v>
+        <f>$D$43*(1+$B$77)^-A98*(1+$B$76)^A98</f>
+        <v>55018243.376348302</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
       <c r="B99" s="26">
-        <f t="shared" si="2"/>
-        <v>49219808.193037339</v>
+        <f>$D$43*(1+$B$77)^-A99*(1+$B$76)^A99</f>
+        <v>54006444.461573519</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100">
-        <f t="shared" si="3"/>
-        <v>26</v>
+        <f t="shared" si="2"/>
+        <v>21</v>
       </c>
       <c r="B100" s="26">
-        <f t="shared" si="2"/>
-        <v>48314643.915536135</v>
+        <f>$D$43*(1+$B$77)^-A100*(1+$B$76)^A100</f>
+        <v>53013252.775621668</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101">
-        <f t="shared" si="3"/>
-        <v>27</v>
+        <f t="shared" si="2"/>
+        <v>22</v>
       </c>
       <c r="B101" s="26">
-        <f t="shared" si="2"/>
-        <v>47426125.829869926</v>
+        <f>$D$43*(1+$B$77)^-A101*(1+$B$76)^A101</f>
+        <v>52038326.127016336</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102">
-        <f t="shared" si="3"/>
-        <v>28</v>
+        <f t="shared" si="2"/>
+        <v>23</v>
       </c>
       <c r="B102" s="26">
-        <f t="shared" si="2"/>
-        <v>46553947.808510877</v>
+        <f>$D$43*(1+$B$77)^-A102*(1+$B$76)^A102</f>
+        <v>51081328.617265843</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103">
-        <f>A102+1</f>
-        <v>29</v>
+        <f t="shared" si="2"/>
+        <v>24</v>
       </c>
       <c r="B103" s="26">
-        <f t="shared" si="2"/>
-        <v>45697809.353690922</v>
+        <f>$D$43*(1+$B$77)^-A103*(1+$B$76)^A103</f>
+        <v>50141930.525133699</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104">
-        <f t="shared" si="3"/>
-        <v>30</v>
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
       <c r="B104" s="26">
-        <f t="shared" si="2"/>
-        <v>44857415.493869409</v>
+        <f>$D$43*(1+$B$77)^-A104*(1+$B$76)^A104</f>
+        <v>49219808.193037339</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105">
-        <f t="shared" si="3"/>
-        <v>31</v>
+        <f t="shared" si="2"/>
+        <v>26</v>
       </c>
       <c r="B105" s="26">
-        <f t="shared" si="2"/>
-        <v>44032476.682104088</v>
+        <f>$D$43*(1+$B$77)^-A105*(1+$B$76)^A105</f>
+        <v>48314643.915536135</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106">
-        <f t="shared" si="3"/>
-        <v>32</v>
+        <f t="shared" si="2"/>
+        <v>27</v>
       </c>
       <c r="B106" s="26">
-        <f t="shared" ref="B106:B134" si="4">$D$43*(1+$B$72)^-A106*(1+$B$71)^A106</f>
-        <v>43222708.69629176</v>
+        <f>$D$43*(1+$B$77)^-A106*(1+$B$76)^A106</f>
+        <v>47426125.829869926</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107">
-        <f t="shared" si="3"/>
-        <v>33</v>
+        <f t="shared" si="2"/>
+        <v>28</v>
       </c>
       <c r="B107" s="26">
-        <f t="shared" si="4"/>
-        <v>42427832.54124289</v>
+        <f>$D$43*(1+$B$77)^-A107*(1+$B$76)^A107</f>
+        <v>46553947.808510877</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108">
-        <f t="shared" si="3"/>
-        <v>34</v>
+        <f>A107+1</f>
+        <v>29</v>
       </c>
       <c r="B108" s="26">
-        <f t="shared" si="4"/>
-        <v>41647574.3525576</v>
+        <f>$D$43*(1+$B$77)^-A108*(1+$B$76)^A108</f>
+        <v>45697809.353690922</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109">
-        <f t="shared" si="3"/>
-        <v>35</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="B109" s="26">
-        <f t="shared" si="4"/>
-        <v>40881665.302269101</v>
+        <f>$D$43*(1+$B$77)^-A109*(1+$B$76)^A109</f>
+        <v>44857415.493869409</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110">
-        <f t="shared" si="3"/>
-        <v>36</v>
+        <f t="shared" si="2"/>
+        <v>31</v>
       </c>
       <c r="B110" s="26">
-        <f t="shared" si="4"/>
-        <v>40129841.506222501</v>
+        <f>$D$43*(1+$B$77)^-A110*(1+$B$76)^A110</f>
+        <v>44032476.682104088</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111">
-        <f t="shared" si="3"/>
-        <v>37</v>
+        <f t="shared" si="2"/>
+        <v>32</v>
       </c>
       <c r="B111" s="26">
-        <f t="shared" si="4"/>
-        <v>39391843.933156848</v>
+        <f t="shared" ref="B111:B139" si="3">$D$43*(1+$B$77)^-A111*(1+$B$76)^A111</f>
+        <v>43222708.69629176</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112">
-        <f t="shared" si="3"/>
-        <v>38</v>
+        <f t="shared" si="2"/>
+        <v>33</v>
       </c>
       <c r="B112" s="26">
-        <f t="shared" si="4"/>
-        <v>38667418.315459296</v>
+        <f t="shared" si="3"/>
+        <v>42427832.54124289</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113">
-        <f t="shared" si="3"/>
-        <v>39</v>
+        <f t="shared" si="2"/>
+        <v>34</v>
       </c>
       <c r="B113" s="26">
-        <f t="shared" si="4"/>
-        <v>37956315.061560355</v>
+        <f t="shared" si="3"/>
+        <v>41647574.3525576</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114">
-        <f t="shared" si="3"/>
-        <v>40</v>
+        <f t="shared" si="2"/>
+        <v>35</v>
       </c>
       <c r="B114" s="26">
-        <f t="shared" si="4"/>
-        <v>37258289.169940449</v>
+        <f t="shared" si="3"/>
+        <v>40881665.302269101</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115">
-        <f t="shared" si="3"/>
-        <v>41</v>
+        <f t="shared" si="2"/>
+        <v>36</v>
       </c>
       <c r="B115" s="26">
-        <f t="shared" si="4"/>
-        <v>36573100.144717649</v>
+        <f t="shared" si="3"/>
+        <v>40129841.506222501</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116">
-        <f>A115+1</f>
-        <v>42</v>
+        <f t="shared" si="2"/>
+        <v>37</v>
       </c>
       <c r="B116" s="26">
-        <f t="shared" si="4"/>
-        <v>35900511.912787966</v>
+        <f t="shared" si="3"/>
+        <v>39391843.933156848</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117">
-        <f t="shared" si="3"/>
-        <v>43</v>
+        <f t="shared" si="2"/>
+        <v>38</v>
       </c>
       <c r="B117" s="26">
-        <f t="shared" si="4"/>
-        <v>35240292.742489375</v>
+        <f t="shared" si="3"/>
+        <v>38667418.315459296</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118">
-        <f t="shared" si="3"/>
-        <v>44</v>
+        <f t="shared" si="2"/>
+        <v>39</v>
       </c>
       <c r="B118" s="26">
-        <f t="shared" si="4"/>
-        <v>34592215.16376166</v>
+        <f t="shared" si="3"/>
+        <v>37956315.061560355</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119">
-        <f>A118+1</f>
-        <v>45</v>
+        <f t="shared" si="2"/>
+        <v>40</v>
       </c>
       <c r="B119" s="26">
-        <f t="shared" si="4"/>
-        <v>33956055.889774427</v>
+        <f t="shared" si="3"/>
+        <v>37258289.169940449</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120">
-        <f t="shared" si="3"/>
-        <v>46</v>
+        <f t="shared" si="2"/>
+        <v>41</v>
       </c>
       <c r="B120" s="26">
-        <f t="shared" si="4"/>
-        <v>33331595.739996634</v>
+        <f t="shared" si="3"/>
+        <v>36573100.144717649</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121">
-        <f t="shared" si="3"/>
-        <v>47</v>
+        <f>A120+1</f>
+        <v>42</v>
       </c>
       <c r="B121" s="26">
-        <f t="shared" si="4"/>
-        <v>32718619.564680599</v>
+        <f t="shared" si="3"/>
+        <v>35900511.912787966</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122">
-        <f t="shared" si="3"/>
-        <v>48</v>
+        <f t="shared" si="2"/>
+        <v>43</v>
       </c>
       <c r="B122" s="26">
-        <f t="shared" si="4"/>
-        <v>32116916.170735013</v>
+        <f t="shared" si="3"/>
+        <v>35240292.742489375</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123">
-        <f t="shared" si="3"/>
-        <v>49</v>
+        <f t="shared" si="2"/>
+        <v>44</v>
       </c>
       <c r="B123" s="26">
-        <f t="shared" si="4"/>
-        <v>31526278.248961017</v>
+        <f t="shared" si="3"/>
+        <v>34592215.16376166</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124">
-        <f t="shared" si="3"/>
-        <v>50</v>
+        <f>A123+1</f>
+        <v>45</v>
       </c>
       <c r="B124" s="26">
-        <f t="shared" si="4"/>
-        <v>30946502.302626465</v>
+        <f t="shared" si="3"/>
+        <v>33956055.889774427</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125">
-        <f t="shared" si="3"/>
-        <v>51</v>
+        <f t="shared" si="2"/>
+        <v>46</v>
       </c>
       <c r="B125" s="26">
-        <f t="shared" si="4"/>
-        <v>30377388.577353776</v>
+        <f t="shared" si="3"/>
+        <v>33331595.739996634</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126">
-        <f t="shared" si="3"/>
-        <v>52</v>
+        <f t="shared" si="2"/>
+        <v>47</v>
       </c>
       <c r="B126" s="26">
-        <f t="shared" si="4"/>
-        <v>29818740.992297079</v>
+        <f t="shared" si="3"/>
+        <v>32718619.564680599</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127">
-        <f t="shared" si="3"/>
-        <v>53</v>
+        <f t="shared" si="2"/>
+        <v>48</v>
       </c>
       <c r="B127" s="26">
-        <f t="shared" si="4"/>
-        <v>29270367.072585084</v>
+        <f t="shared" si="3"/>
+        <v>32116916.170735013</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128">
-        <f t="shared" si="3"/>
-        <v>54</v>
+        <f t="shared" si="2"/>
+        <v>49</v>
       </c>
       <c r="B128" s="26">
-        <f t="shared" si="4"/>
-        <v>28732077.883006334</v>
+        <f t="shared" si="3"/>
+        <v>31526278.248961017</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129">
-        <f t="shared" si="3"/>
-        <v>55</v>
+        <f t="shared" si="2"/>
+        <v>50</v>
       </c>
       <c r="B129" s="26">
-        <f t="shared" si="4"/>
-        <v>28203687.962913968</v>
+        <f t="shared" si="3"/>
+        <v>30946502.302626465</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130">
-        <f t="shared" si="3"/>
-        <v>56</v>
+        <f t="shared" si="2"/>
+        <v>51</v>
       </c>
       <c r="B130" s="26">
-        <f t="shared" si="4"/>
-        <v>27685015.262327705</v>
+        <f t="shared" si="3"/>
+        <v>30377388.577353776</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131">
-        <f t="shared" si="3"/>
-        <v>57</v>
+        <f t="shared" si="2"/>
+        <v>52</v>
       </c>
       <c r="B131" s="26">
-        <f t="shared" si="4"/>
-        <v>27175881.079210754</v>
+        <f t="shared" si="3"/>
+        <v>29818740.992297079</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132">
-        <f>A131+1</f>
-        <v>58</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="B132" s="26">
-        <f t="shared" si="4"/>
-        <v>26676109.997900393</v>
+        <f t="shared" si="3"/>
+        <v>29270367.072585084</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133">
-        <f t="shared" si="3"/>
-        <v>59</v>
+        <f t="shared" si="2"/>
+        <v>54</v>
       </c>
       <c r="B133" s="26">
-        <f t="shared" si="4"/>
-        <v>26185529.82867071</v>
+        <f t="shared" si="3"/>
+        <v>28732077.883006334</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="B134" s="26">
+        <f t="shared" si="3"/>
+        <v>28203687.962913968</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="B135" s="26">
+        <f t="shared" si="3"/>
+        <v>27685015.262327705</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="B136" s="26">
+        <f t="shared" si="3"/>
+        <v>27175881.079210754</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <f>A136+1</f>
+        <v>58</v>
+      </c>
+      <c r="B137" s="26">
+        <f t="shared" si="3"/>
+        <v>26676109.997900393</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="B138" s="26">
+        <f t="shared" si="3"/>
+        <v>26185529.82867071</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="B134" s="26">
-        <f t="shared" si="4"/>
+      <c r="B139" s="26">
+        <f t="shared" si="3"/>
         <v>25703971.548406877</v>
       </c>
     </row>
@@ -3028,8 +3082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60C3FA1-C501-488F-99EF-B28CB9021ECA}">
   <dimension ref="A1:R131"/>
   <sheetViews>
-    <sheetView zoomScale="112" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView topLeftCell="A35" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3769,7 +3823,7 @@
         <v>50</v>
       </c>
       <c r="C49">
-        <f t="dataTable" ref="C49:C50" dt2D="0" dtr="0" r1="H20" ca="1"/>
+        <f t="dataTable" ref="C49:C50" dt2D="0" dtr="0" r1="H20"/>
         <v>0.21645872623574136</v>
       </c>
       <c r="D49" t="s">
@@ -3877,7 +3931,7 @@
         <v>1.9789999999999999E-2</v>
       </c>
       <c r="E61">
-        <f t="dataTable" ref="E61:G63" dt2D="1" dtr="1" r1="H20" r2="Q26"/>
+        <f t="dataTable" ref="E61:G63" dt2D="1" dtr="1" r1="H20" r2="Q26" ca="1"/>
         <v>0.27115659695817496</v>
       </c>
       <c r="F61">

</xml_diff>